<commit_message>
add dvd insert function
</commit_message>
<xml_diff>
--- a/DVD/res/design/res/testSample/dvd_test_sample.xlsx
+++ b/DVD/res/design/res/testSample/dvd_test_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qkdlf\Project\back-end\DVD_ManagementSystem\DVD\res\design\res\testSample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEC70BF-C3E7-44DD-83CA-1DCC235F592B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C023E3DD-C788-4669-8337-71585B030731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{523C9EEB-31AC-4B25-B256-CA254B3682C9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>D_NUM</t>
   </si>
@@ -98,18 +98,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전체</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>전쟁/드라마</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>15세 이상</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>나홍진</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -118,10 +110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>19세 이상</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>하울의 움직이는 성</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -171,10 +159,6 @@
   </si>
   <si>
     <t>판타지/드라마</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12세 이상</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -593,7 +577,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -613,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -650,8 +634,8 @@
       <c r="F2" s="1">
         <v>2000</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
@@ -668,13 +652,13 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1">
         <v>2500</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
+      <c r="G3">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -682,7 +666,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2">
         <v>39492</v>
@@ -691,13 +675,13 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1">
         <v>2500</v>
       </c>
-      <c r="G4" t="s">
-        <v>22</v>
+      <c r="G4">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -705,22 +689,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2">
         <v>38345</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1">
         <v>2500</v>
       </c>
-      <c r="G5" t="s">
-        <v>17</v>
+      <c r="G5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -728,22 +712,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2">
         <v>43615</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1">
         <v>2500</v>
       </c>
-      <c r="G6" t="s">
-        <v>19</v>
+      <c r="G6">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
@@ -751,7 +735,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2">
         <v>38611</v>
@@ -760,13 +744,13 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1">
         <v>2500</v>
       </c>
-      <c r="G7" t="s">
-        <v>17</v>
+      <c r="G7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -774,7 +758,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2">
         <v>44420</v>
@@ -783,13 +767,13 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1">
         <v>2500</v>
       </c>
-      <c r="G8" t="s">
-        <v>19</v>
+      <c r="G8">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -797,7 +781,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2">
         <v>44377</v>
@@ -806,13 +790,13 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1">
         <v>2500</v>
       </c>
-      <c r="G9" t="s">
-        <v>36</v>
+      <c r="G9">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -820,7 +804,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2">
         <v>44384</v>
@@ -829,13 +813,13 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F10" s="1">
         <v>2500</v>
       </c>
-      <c r="G10" t="s">
-        <v>36</v>
+      <c r="G10">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
@@ -843,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2">
         <v>41025</v>
@@ -852,13 +836,13 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F11" s="1">
         <v>2500</v>
       </c>
-      <c r="G11" t="s">
-        <v>36</v>
+      <c r="G11">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>